<commit_message>
updated alz network templates
</commit_message>
<xml_diff>
--- a/102-Azure-Landing-Zones/docs/Azure Network Documentation Template.xlsx
+++ b/102-Azure-Landing-Zones/docs/Azure Network Documentation Template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26125"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/jovella_microsoft_com/Documents/Git/what-the-caf/learning_path_modules/04_ALZ_Accelerator/sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsofteur-my.sharepoint.com/personal/jovella_microsoft_com/Documents/Scripts/Azure Networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{E489F088-6B2F-471E-B231-1A059A82CF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F169EE25-D402-45B3-B34C-A13F0C413A54}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{33D46CD7-BC3C-4ABA-9A2E-0946D4AA22C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" tabRatio="554" xr2:uid="{C820F456-7308-4348-96BC-0FE680A270E1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{63E1118A-84D6-4246-847F-D559ABD8C16F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IP Address Planning" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,57 +36,171 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+  <si>
+    <t>VNET Name</t>
+  </si>
+  <si>
+    <t>Address Space</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Workload</t>
+  </si>
+  <si>
+    <t>Windows Server ADDS</t>
+  </si>
+  <si>
+    <t>Azure Bastion</t>
+  </si>
+  <si>
+    <t>Azure Firewall, Azure VPN Gateway</t>
+  </si>
   <si>
     <t>Subnet Name</t>
   </si>
   <si>
-    <t>VNET Name</t>
-  </si>
-  <si>
-    <t>VNET Address Space</t>
-  </si>
-  <si>
-    <t>Subnet Address Space</t>
-  </si>
-  <si>
-    <t>vnet-hub-weu001</t>
-  </si>
-  <si>
-    <t>10.0.0.0/26</t>
-  </si>
-  <si>
-    <t>Service Deployed</t>
-  </si>
-  <si>
-    <t>NSG</t>
-  </si>
-  <si>
-    <t>UDR</t>
-  </si>
-  <si>
-    <t>Documentation</t>
-  </si>
-  <si>
-    <t>Azure Firewall FAQ | Microsoft Docs</t>
+    <t>Subnet Size</t>
+  </si>
+  <si>
+    <t>Subnet Address</t>
+  </si>
+  <si>
+    <t>/26</t>
+  </si>
+  <si>
+    <t>/27</t>
+  </si>
+  <si>
+    <t>GatewaySubnet</t>
   </si>
   <si>
     <t>AzureFirewallSubnet</t>
   </si>
   <si>
-    <t>Firewall</t>
-  </si>
-  <si>
-    <t>AzureBastion</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Bastion</t>
-  </si>
-  <si>
-    <t>Gateway</t>
+    <t>AzureFirewallManagementSubnet</t>
+  </si>
+  <si>
+    <t>Recommended Size</t>
+  </si>
+  <si>
+    <t>/24</t>
+  </si>
+  <si>
+    <t>/23</t>
+  </si>
+  <si>
+    <t>AzureBastionSubnet</t>
+  </si>
+  <si>
+    <t>AddsSubnet</t>
+  </si>
+  <si>
+    <t>WafSubnet</t>
+  </si>
+  <si>
+    <t>WebSubnet</t>
+  </si>
+  <si>
+    <t>ApiSubnet</t>
+  </si>
+  <si>
+    <t>DbSubnet</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Azure VPN Gateway</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>PIP Name</t>
+  </si>
+  <si>
+    <t>PIP Value</t>
+  </si>
+  <si>
+    <t>Local Gateway</t>
+  </si>
+  <si>
+    <t>BGP</t>
+  </si>
+  <si>
+    <t>Zonal</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Local LAN</t>
+  </si>
+  <si>
+    <t>Remote LAN</t>
+  </si>
+  <si>
+    <t>On-Premises</t>
+  </si>
+  <si>
+    <t>vpn-hub-eus01</t>
+  </si>
+  <si>
+    <t>East US</t>
+  </si>
+  <si>
+    <t>alz</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>vnet-hub-eus01</t>
+  </si>
+  <si>
+    <t>vnet-bst-eus01</t>
+  </si>
+  <si>
+    <t>vnet-sharedsvc-eus01</t>
+  </si>
+  <si>
+    <t>vnet-prod-wload-eus01</t>
+  </si>
+  <si>
+    <t>Address Space dedicated to Azure East US region</t>
+  </si>
+  <si>
+    <t>10.0.0.0/16</t>
+  </si>
+  <si>
+    <t>10.0.0.0/24</t>
+  </si>
+  <si>
+    <t>10.0.1.0/24</t>
+  </si>
+  <si>
+    <t>10.0.3.0/23</t>
+  </si>
+  <si>
+    <t>10.0.2.0/24</t>
+  </si>
+  <si>
+    <t>pip-vpn-hub-eus01</t>
+  </si>
+  <si>
+    <t>pip-vpn-hub-eus02</t>
+  </si>
+  <si>
+    <t>Peerings</t>
   </si>
 </sst>
 </file>
@@ -97,7 +211,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -105,15 +219,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -139,16 +251,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -178,39 +283,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -262,7 +367,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -373,13 +478,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -388,6 +486,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -452,124 +557,438 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3A99E0-BDF6-4077-AD11-335A99E92C0A}">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F5CC69-1419-4CD5-9C10-44170587F180}">
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="198" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.87890625" customWidth="1"/>
-    <col min="2" max="2" width="17.9375" customWidth="1"/>
-    <col min="3" max="3" width="22.1171875" customWidth="1"/>
-    <col min="4" max="4" width="20.703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5859375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.26953125" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="51.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F10" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="G10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
-        <v>4</v>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="D41" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="https://docs.microsoft.com/en-us/azure/firewall/firewall-faq" xr:uid="{BCD81901-FB6C-41E8-ABE5-49D8260F4149}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
-  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>